<commit_message>
EI Variable Installments T1 scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3110-MS-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-INSTALLMENT-FEE-FLAT-Regular-CASH-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/3110-MS-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-INSTALLMENT-FEE-FLAT-Regular-CASH-Makerepayment1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="5" r:id="rId1"/>
@@ -298,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -307,9 +307,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -648,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -659,26 +656,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>42036</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>987.72</v>
       </c>
     </row>
@@ -692,7 +689,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD13"/>
+      <selection activeCell="A8" sqref="A8:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,85 +724,85 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>10000</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>785.8</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
         <v>9214.2000000000007</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>802.9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>668.41</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>101.92</v>
       </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
         <v>566.49</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>84.82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>1200</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>100</v>
       </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
         <v>1100</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>0</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="A5" s="7">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -818,7 +815,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD16"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,547 +889,547 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8">
         <v>42005</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="9">
         <v>10000</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8">
-        <v>0</v>
-      </c>
-      <c r="L2" s="8">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>31</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>42036</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>42036</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="8">
+      <c r="E3" s="11"/>
+      <c r="F3" s="7">
         <v>785.8</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>9214.2000000000007</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>101.92</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>100</v>
       </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L3" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L3" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>28</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>42064</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7">
         <v>802.9</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>8411.2999999999993</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>84.82</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>100</v>
       </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L4" s="8">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
-      <c r="P4" s="8">
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>31</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>42095</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7">
         <v>793.81</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>7617.49</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>93.91</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>100</v>
       </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
-        <v>0</v>
-      </c>
-      <c r="N5" s="8">
-        <v>0</v>
-      </c>
-      <c r="P5" s="8">
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>30</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>42125</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
         <v>812.59</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <v>6804.9</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>75.13</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>100</v>
       </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L6" s="8">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
-        <v>0</v>
-      </c>
-      <c r="N6" s="8">
-        <v>0</v>
-      </c>
-      <c r="P6" s="8">
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>31</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>42156</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7">
         <v>818.37</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>5986.53</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>69.349999999999994</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>100</v>
       </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L7" s="8">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8">
-        <v>0</v>
-      </c>
-      <c r="P7" s="8">
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>30</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>42186</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7">
         <v>828.67</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>5157.8599999999997</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>59.05</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>100</v>
       </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L8" s="8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="8">
-        <v>0</v>
-      </c>
-      <c r="P8" s="8">
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>31</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>42217</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7">
         <v>835.15</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <v>4322.71</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>52.57</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>100</v>
       </c>
-      <c r="J9" s="8">
-        <v>0</v>
-      </c>
-      <c r="K9" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L9" s="8">
-        <v>0</v>
-      </c>
-      <c r="M9" s="8">
-        <v>0</v>
-      </c>
-      <c r="N9" s="8">
-        <v>0</v>
-      </c>
-      <c r="P9" s="8">
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>31</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>42248</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7">
         <v>843.66</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>3479.05</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>44.06</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>100</v>
       </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L10" s="8">
-        <v>0</v>
-      </c>
-      <c r="M10" s="8">
-        <v>0</v>
-      </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
-      <c r="P10" s="8">
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7">
+        <v>0</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>30</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>42278</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7">
         <v>853.41</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>2625.64</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>34.31</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>100</v>
       </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L11" s="8">
-        <v>0</v>
-      </c>
-      <c r="M11" s="8">
-        <v>0</v>
-      </c>
-      <c r="N11" s="8">
-        <v>0</v>
-      </c>
-      <c r="P11" s="8">
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>31</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>42309</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7">
         <v>860.96</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>1764.68</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>26.76</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>100</v>
       </c>
-      <c r="J12" s="8">
-        <v>0</v>
-      </c>
-      <c r="K12" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L12" s="8">
-        <v>0</v>
-      </c>
-      <c r="M12" s="8">
-        <v>0</v>
-      </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
-      <c r="P12" s="8">
+      <c r="J12" s="7">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>30</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>42339</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
         <v>870.31</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>894.37</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>17.41</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>100</v>
       </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="L13" s="8">
-        <v>0</v>
-      </c>
-      <c r="M13" s="8">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
-      <c r="P13" s="8">
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
+        <v>0</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
         <v>987.72</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>31</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>42370</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7">
         <v>894.37</v>
       </c>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-      <c r="H14" s="8">
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
         <v>9.1199999999999992</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>100</v>
       </c>
-      <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="J14" s="7">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
         <v>1003.49</v>
       </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="8">
-        <v>0</v>
-      </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="P14" s="11">
+      <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7">
+        <v>0</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
         <v>1003.49</v>
       </c>
     </row>
@@ -1447,7 +1444,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A4" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,70 +1495,72 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>216</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="7">
+        <v>135</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>42036</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="8">
-        <v>987.72</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="E2" s="7">
+        <v>987.72</v>
+      </c>
+      <c r="F2" s="7">
         <v>785.8</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>101.92</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>100</v>
       </c>
-      <c r="I2" s="8">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11">
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10">
         <v>9214.2000000000007</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>213</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="7">
+        <v>132</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>42005</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>10000</v>
       </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="10">
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9">
         <v>10000</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1572,38 +1571,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1614,7 +1623,7 @@
       <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <v>42005</v>
       </c>
       <c r="D2" t="s">
@@ -1640,7 +1649,7 @@
       <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>42005</v>
       </c>
       <c r="D3" t="s">
@@ -1674,51 +1683,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="14"/>
-    <col min="2" max="2" width="17" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="14"/>
-    <col min="7" max="7" width="21.85546875" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="17" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="13"/>
+    <col min="7" max="7" width="21.85546875" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <v>42036</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1733,18 +1742,18 @@
       <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>42036</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1759,18 +1768,18 @@
       <c r="G3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>42036</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1785,18 +1794,18 @@
       <c r="G4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>42036</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1811,7 +1820,7 @@
       <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>